<commit_message>
Split the total process into multiple small processes
</commit_message>
<xml_diff>
--- a/FixedAssertTest/AssetsPurchase/data/EstatePlanning.xlsx
+++ b/FixedAssertTest/AssetsPurchase/data/EstatePlanning.xlsx
@@ -36,10 +36,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>信息化部</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>规划类型</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -143,6 +139,10 @@
   </si>
   <si>
     <t>规格型号6</t>
+  </si>
+  <si>
+    <t>检测站</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -506,7 +506,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -540,38 +540,38 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -581,33 +581,33 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -616,18 +616,18 @@
         <v>1000</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>26</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -636,18 +636,18 @@
         <v>1050</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -656,18 +656,18 @@
         <v>1100</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -676,18 +676,18 @@
         <v>1150</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -696,18 +696,18 @@
         <v>1200</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -716,7 +716,7 @@
         <v>1250</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>